<commit_message>
remove high tolerance results files from Reported_results; update results file for Model B rep 2 low tolerance; change model objective order in Analysis_Plots to match paper
</commit_message>
<xml_diff>
--- a/Reported_results/ModelB_PEM_rep2_lowtol/PARAMETER ESTIMATION rep2 slice drop high error/OPT RESULTS.xlsx
+++ b/Reported_results/ModelB_PEM_rep2_lowtol/PARAMETER ESTIMATION rep2 slice drop high error/OPT RESULTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdreyer/Documents/Github/COVID_Dx_GAMES/Results/230920_ModelB_PEM_rep2_lowtol/PARAMETER ESTIMATION rep2 slice drop high error/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdreyer/Documents/Github/COVID_Dx_GAMES/Reported_results/ModelB_PEM_rep2_lowtol/PARAMETER ESTIMATION rep2 slice drop high error/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958912D8-4B75-834A-978B-561156003A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74447834-D011-714B-949F-C4D70B8ADCF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="4180" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,21 +271,15 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -308,19 +302,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -623,15 +629,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X25"/>
+  <dimension ref="A1:Z25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X21" sqref="A21:X21"/>
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,8 +707,9 @@
       <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -776,7 +783,7 @@
         <v>0.27287795627333777</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>21</v>
       </c>
@@ -850,7 +857,7 @@
         <v>0.2644035258443399</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -924,7 +931,7 @@
         <v>0.28077538358780729</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>19</v>
       </c>
@@ -998,7 +1005,7 @@
         <v>0.28444341387464778</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>18</v>
       </c>
@@ -1072,7 +1079,7 @@
         <v>0.26843136969336368</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>17</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>0.28357013906008482</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>16</v>
       </c>
@@ -1220,7 +1227,7 @@
         <v>0.27271547505577809</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>15</v>
       </c>
@@ -1294,7 +1301,7 @@
         <v>0.27233586292363388</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>14</v>
       </c>
@@ -1368,7 +1375,7 @@
         <v>0.27193535666538182</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>13</v>
       </c>
@@ -1442,7 +1449,7 @@
         <v>0.27872446244946558</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>12</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>0.28459320225484469</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1590,7 +1597,7 @@
         <v>0.30047391029124582</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>10</v>
       </c>
@@ -1664,7 +1671,7 @@
         <v>0.26276926922350252</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -1738,7 +1745,7 @@
         <v>0.30225414034055692</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>8</v>
       </c>
@@ -2109,76 +2116,76 @@
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="3">
         <v>3</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>1.5301467090009859E-4</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="4">
         <v>169.78715038407469</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="4">
         <v>0.36192884708449252</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="4">
         <v>21.237418181483839</v>
       </c>
-      <c r="F21" s="3">
+      <c r="F21" s="4">
         <v>9.77049436385206E-2</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G21" s="4">
         <v>100.71016280864779</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>87.793954484660617</v>
       </c>
-      <c r="I21" s="3">
-        <v>1</v>
-      </c>
-      <c r="J21" s="3">
+      <c r="I21" s="4">
+        <v>1</v>
+      </c>
+      <c r="J21" s="4">
         <v>5.6310714914318569E-5</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="4">
         <v>6474.4682647735081</v>
       </c>
-      <c r="L21" s="3">
+      <c r="L21" s="4">
         <v>3.6358361409898322E-2</v>
       </c>
-      <c r="M21" s="3">
+      <c r="M21" s="4">
         <v>233.01245922571519</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="4">
         <v>0.1388304686119457</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="4">
         <v>47.511422150239213</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="4">
         <v>55.223347844654462</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="R21" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="S21" s="3">
+      <c r="R21" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S21" s="4">
         <v>2</v>
       </c>
-      <c r="T21" s="3" t="s">
+      <c r="T21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="U21" s="3" t="s">
+      <c r="U21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="V21" s="3" t="s">
+      <c r="V21" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="W21" s="3" t="s">
+      <c r="W21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="X21" s="3">
+      <c r="X21" s="4">
         <v>0.31033969862594918</v>
       </c>
     </row>

</xml_diff>